<commit_message>
Reverted to use of iNat ids because of Neovison vison revision. Added filtering for some duplicate obs from iNat and PMLS. Reacquired iNaturalist observations and taxa. Resolved reviewer feedback on "sex" column. Regenerated visualisation files.
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Mammalia.xlsx
+++ b/data/dataPaper-I-in/arphified/Mammalia.xlsx
@@ -267,13 +267,13 @@
     <t>(Schreber, 1777)</t>
   </si>
   <si>
-    <t>74758</t>
+    <t>1264432</t>
   </si>
   <si>
     <t>Mustelinae</t>
   </si>
   <si>
-    <t>Neovison</t>
+    <t>Neogale</t>
   </si>
   <si>
     <t>vison</t>

</xml_diff>